<commit_message>
add ubike and bus info
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="11985" windowHeight="7725" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -419,13 +419,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
+  <cols>
+    <col width="37.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="37.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="27.28515625" bestFit="1" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1235,7 +1241,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2022-05-07 20:21:03.801000</t>
+          <t>2022-05-08 20:54:41.028000</t>
         </is>
       </c>
     </row>
@@ -1247,17 +1253,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>訂購</t>
+          <t>bus 你好</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>nontextreply</t>
+          <t>桃園公車中查無此資料</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2022-05-07 20:21:22.911000</t>
+          <t>2022-05-08 20:58:06.508000</t>
         </is>
       </c>
     </row>
@@ -1269,17 +1275,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>訂購</t>
+          <t>ubike 哈哈</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>nontextreply</t>
+          <t>桃園ubike中查無此資料</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2022-05-07 20:23:05.931000</t>
+          <t>2022-05-08 20:58:22.101000</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1297,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>我要購買</t>
+          <t>鋼筆多少</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>鋼筆 30元</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2022-05-07 20:23:13.172000</t>
+          <t>2022-05-08 21:00:10.521000</t>
         </is>
       </c>
     </row>
@@ -1308,17 +1319,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>請問營業時間</t>
+          <t>怎麼購買</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>每日AM 11:00~ PM 7:00 禮拜三公休</t>
+          <t>nontextreply</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2022-05-07 20:24:04.747000</t>
+          <t>2022-05-08 21:00:28.830000</t>
         </is>
       </c>
     </row>
@@ -1330,12 +1341,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>如何購買</t>
+          <t>bus 健行科技大學</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>桃園公車中查無此資料</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2022-05-07 20:24:12.339000</t>
+          <t>2022-05-08 21:01:03.663000</t>
         </is>
       </c>
     </row>
@@ -1347,17 +1363,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>馬克杯多少錢</t>
+          <t>ubike 健行科技大學</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>馬克杯 100元</t>
+          <t>中文場站名稱:健行科技大學
+場站總停車格:66
+場站目前車輛數:34
+地址:健行路229號(商學大樓後人行道)
+場站是否暫停營運1</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2022-05-07 20:26:29.829000</t>
+          <t>2022-05-08 21:01:22.431000</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1389,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>我帥嗎</t>
+          <t>Bus 171-FS</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1379,7 +1399,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2022-05-07 20:26:36.706000</t>
+          <t>2022-05-08 21:12:24.115000</t>
         </is>
       </c>
     </row>
@@ -1391,12 +1411,21 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>我要購買</t>
+          <t xml:space="preserve">bus 171-FS </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>車輛:171-FS
+業者代號:45
+GPS車速:0.0
+GPS時間:2022-05-07 22:15:26
+路線方向(1:去程,2:回程):1</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2022-05-07 20:26:44.059000</t>
+          <t>2022-05-08 21:12:45.175000</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1437,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>我要訂購</t>
+          <t>位置在哪</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1418,7 +1447,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2022-05-07 20:29:58.543000</t>
+          <t>2022-05-08 21:22:06.813000</t>
         </is>
       </c>
     </row>
@@ -1430,17 +1459,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>填寫表單</t>
+          <t>位置</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://forms.gle/vdHfmWijtcBTsPNX6</t>
+          <t>nontextreply</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2022-05-07 20:30:10.798000</t>
+          <t>2022-05-08 21:22:44.916000</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1481,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>我要購買</t>
+          <t>位置呢</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1462,7 +1491,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2022-05-08 15:31:17.539000</t>
+          <t>2022-05-08 21:23:01.917000</t>
         </is>
       </c>
     </row>
@@ -1474,17 +1503,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>我要訂購</t>
+          <t>地址是？</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>nontextreply</t>
+          <t>261宜蘭縣頭城鎮港口路92-1號</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2022-05-08 15:31:32.853000</t>
+          <t>2022-05-08 21:23:29.902000</t>
         </is>
       </c>
     </row>
@@ -1496,149 +1525,21 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>表單怎麼填</t>
+          <t>ubike 健行科技大學</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Unable to recognize user's input</t>
+          <t>中文場站名稱:健行科技大學
+場站總停車格:66
+場站目前車輛數:34
+地址:健行路229號(商學大樓後人行道)
+場站是否暫停營運1</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2022-05-08 15:31:44.535000</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>U53e8616065a61b190a510f520198a271</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>表單</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Unable to recognize user's input</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>2022-05-08 15:32:03.332000</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>U53e8616065a61b190a510f520198a271</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>表單</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>https://forms.gle/vdHfmWijtcBTsPNX6</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>2022-05-08 15:35:12.980000</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>U53e8616065a61b190a510f520198a271</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>表單怎麼填</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>https://forms.gle/vdHfmWijtcBTsPNX6</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>2022-05-08 15:35:21.727000</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>U53e8616065a61b190a510f520198a271</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>有表單嗎</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>https://forms.gle/vdHfmWijtcBTsPNX6</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>2022-05-08 15:35:27.873000</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>U53e8616065a61b190a510f520198a271</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>地址</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>261宜蘭縣頭城鎮港口路92-1號</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>2022-05-08 15:35:55.369000</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>U53e8616065a61b190a510f520198a271</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>我想購買</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>nontextreply</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>2022-05-08 15:38:35.201000</t>
+          <t>2022-05-08 21:25:29.317000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add bus location present
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
@@ -1543,6 +1543,450 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>bus KKA-8155</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>車輛:KKA-8155
+業者代號:34
+GPS車速:98.0
+GPS時間:2022-05-09 11:18:59
+路線方向(1:去程,2:回程):1</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2022-05-09 22:19:29.557000</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>bus KKA-8155</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>車輛:KKA-8155
+業者代號:34
+GPS車速:98.0
+GPS時間:2022-05-09 11:18:59
+路線方向(1:去程,2:回程):1</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2022-05-09 22:22:56.174000</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>bus fuck</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2022-05-09 22:25:34.543000</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>bus KKA-8155</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>車輛:KKA-8155
+業者代號:34
+GPS車速:98.0
+GPS時間:2022-05-09 11:18:59
+路線方向(1:去程,2:回程):1</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2022-05-09 22:41:54.154000</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>bus. 123</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2022-05-09 22:42:35.137000</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>bus 123</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>桃園公車中查無此資料</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:29:19.487000</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>筆記本</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>筆記本50元</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:29:29.618000</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>地址</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>261宜蘭縣頭城鎮港口路92-1號</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:29:53.618000</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ubike 健行科技大學</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>中文場站名稱:健行科技大學
+場站總停車格:66
+場站目前車輛數:15
+地址:健行路229號(商學大樓後人行道)
+場站是否暫停營運1</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:30:08.741000</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ubike 健行科技大學</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>中文場站名稱:健行科技大學
+場站總停車格:66
+場站目前車輛數:15
+地址:健行路229號(商學大樓後人行道)
+場站是否暫停營運1</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:53:14.429000</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ubike 健行科技大學</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>中文場站名稱:健行科技大學
+場站總停車格:66
+場站目前車輛數:15
+地址:健行路229號(商學大樓後人行道)
+場站是否暫停營運1</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:55:03.262000</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>地址</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>261宜蘭縣頭城鎮港口路92-1號</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:55:29.282000</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>bus KKA-8155</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>車輛:KKA-8155
+業者代號:34
+GPS車速:98.0
+GPS時間:2022-05-09 11:18:59
+路線方向(1:去程,2:回程):1</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:55:43.636000</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>我</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Unable to recognize user's input</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2022-05-10 09:58:55.522000</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>地址</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>261宜蘭縣頭城鎮港口路92-1號</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2022-05-10 10:48:39.557000</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>ubike 健行科技大學</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>中文場站名稱:健行科技大學
+場站總停車格:66
+場站目前車輛數:15
+地址:健行路229號(商學大樓後人行道)
+場站是否暫停營運1</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2022-05-10 10:48:51.925000</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>bus KKA-8155</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>車輛:KKA-8155
+業者代號:34
+GPS車速:98.0
+GPS時間:2022-05-09 11:18:59
+路線方向(1:去程,2:回程):1</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2022-05-10 10:49:05.773000</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>有表單嗎</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://forms.gle/vdHfmWijtcBTsPNX6</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2022-05-10 10:55:14.876000</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>U53e8616065a61b190a510f520198a271</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>位置情報</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>nontextreply</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2022-05-10 11:23:50.980000</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>